<commit_message>
Utilities added , code optimization, Support - iOS Checker
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testData_Checker.xlsx
+++ b/src/main/resources/dataSheets/testData_Checker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23325" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23325" windowHeight="7770" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="19" r:id="rId1"/>
@@ -624,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>